<commit_message>
slimmed down pipeline files
</commit_message>
<xml_diff>
--- a/PipelineRunDetails.xlsx
+++ b/PipelineRunDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evamorrison/Desktop/Eva/fullWorkflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088F230E-4C2B-9646-87BB-9D5175504F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F805C4-DA2F-BA48-BC32-376918DC6941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{1570BB8B-16E4-774E-86B1-BEA8F2160844}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>TE</t>
   </si>
@@ -110,6 +110,102 @@
   </si>
   <si>
     <t>9.extended.bed</t>
+  </si>
+  <si>
+    <t>sequences</t>
+  </si>
+  <si>
+    <t>lines</t>
+  </si>
+  <si>
+    <t>file size</t>
+  </si>
+  <si>
+    <t>247 KB</t>
+  </si>
+  <si>
+    <t>254.6 KB</t>
+  </si>
+  <si>
+    <t>247.8 KB</t>
+  </si>
+  <si>
+    <t>255 KB</t>
+  </si>
+  <si>
+    <t>28.7 KB</t>
+  </si>
+  <si>
+    <t>21.5 KB</t>
+  </si>
+  <si>
+    <t>26.9 KB</t>
+  </si>
+  <si>
+    <t>33.7 KB</t>
+  </si>
+  <si>
+    <t>33.9 KB</t>
+  </si>
+  <si>
+    <t>56.3 KB</t>
+  </si>
+  <si>
+    <t>69.0 KB</t>
+  </si>
+  <si>
+    <t>56.1 KB</t>
+  </si>
+  <si>
+    <t>68.8 KB</t>
+  </si>
+  <si>
+    <t>40.0 KB</t>
+  </si>
+  <si>
+    <t>53.4 KB</t>
+  </si>
+  <si>
+    <t>39.9 KB</t>
+  </si>
+  <si>
+    <t>65.8 KB</t>
+  </si>
+  <si>
+    <t>74.8 KB</t>
+  </si>
+  <si>
+    <t>74.6 KB</t>
+  </si>
+  <si>
+    <t>24.3 KB</t>
+  </si>
+  <si>
+    <t>30.6 KB</t>
+  </si>
+  <si>
+    <t>24.2 KB</t>
+  </si>
+  <si>
+    <t>30.3 KB</t>
+  </si>
+  <si>
+    <t>8.4 KB</t>
+  </si>
+  <si>
+    <t>8.8 KB</t>
+  </si>
+  <si>
+    <t>8.3 KB</t>
+  </si>
+  <si>
+    <t>8.7 KB</t>
+  </si>
+  <si>
+    <t>1.6 KB</t>
+  </si>
+  <si>
+    <t>8.1 KB</t>
   </si>
 </sst>
 </file>
@@ -157,10 +253,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E84438F-10C5-5B47-B2BF-9C90F5B1433D}">
-  <dimension ref="B2:Q11"/>
+  <dimension ref="B1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,99 +597,533 @@
     <col min="16" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="C3">
+        <v>230</v>
+      </c>
+      <c r="D3">
+        <v>8338</v>
+      </c>
+      <c r="E3">
+        <v>8666</v>
+      </c>
+      <c r="F3">
+        <v>440</v>
+      </c>
+      <c r="G3">
+        <v>413</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3">
+        <v>62</v>
+      </c>
+      <c r="M3">
+        <v>65</v>
+      </c>
+      <c r="N3">
+        <v>8338</v>
+      </c>
+      <c r="O3">
+        <v>8666</v>
+      </c>
+      <c r="P3">
+        <v>33</v>
+      </c>
+      <c r="Q3">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>41</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>214</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>214</v>
+      </c>
+      <c r="O5">
+        <v>68</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C6">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>288</v>
+      </c>
+      <c r="E6">
+        <v>269</v>
+      </c>
+      <c r="F6">
+        <v>118</v>
+      </c>
+      <c r="G6">
+        <v>119</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="M6">
+        <v>17</v>
+      </c>
+      <c r="N6">
+        <v>288</v>
+      </c>
+      <c r="O6">
+        <v>269</v>
+      </c>
+      <c r="P6">
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>277</v>
+      </c>
+      <c r="E7">
+        <v>965</v>
+      </c>
+      <c r="F7">
+        <v>162</v>
+      </c>
+      <c r="G7">
+        <v>725</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7">
+        <v>22</v>
+      </c>
+      <c r="M7">
+        <v>27</v>
+      </c>
+      <c r="N7">
+        <v>277</v>
+      </c>
+      <c r="O7">
+        <v>965</v>
+      </c>
+      <c r="P7">
+        <v>15</v>
+      </c>
+      <c r="Q7">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>254</v>
+      </c>
+      <c r="E8">
+        <v>389</v>
+      </c>
+      <c r="F8">
+        <v>109</v>
+      </c>
+      <c r="G8">
+        <v>117</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8">
+        <v>21</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+      <c r="N8">
+        <v>254</v>
+      </c>
+      <c r="O8">
+        <v>389</v>
+      </c>
+      <c r="P8">
+        <v>16</v>
+      </c>
+      <c r="Q8">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>82</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>82</v>
+      </c>
+      <c r="O9">
+        <v>55</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <v>34</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>53</v>
+      </c>
+      <c r="O10">
+        <v>34</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>